<commit_message>
Moved to different location.
</commit_message>
<xml_diff>
--- a/P05/Scrum_MICE.xlsx
+++ b/P05/Scrum_MICE.xlsx
@@ -574,42 +574,10 @@
     <t xml:space="preserve">-Create MixInFlavor; super constructor’s arguments to parent Item</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-Create MixIn and MixInAmount; MixIn contains both a MixInFlavor </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">and MixInAmount, MixIn.toString() returns those values for use</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-Create Scoop; contains a MixIn and IceCreamFlavor. .toString() </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">returns flavor with a list of MixIns [can be added via addMixin()]</t>
-    </r>
+    <t xml:space="preserve">-Create MixIn and MixInAmount; MixIn contains both a MixInFlavor and MixInAmount, MixIn.toString() returns those values for use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Create Scoop; contains a MixIn and IceCreamFlavor. .toString() returns flavor with a list of MixIns [can be added via addMixin()]. Regression test for functionality.</t>
   </si>
   <si>
     <t xml:space="preserve">MixIn list has an unwanted space preceding it</t>
@@ -634,7 +602,7 @@
     <numFmt numFmtId="166" formatCode="mmm\ dd"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -748,11 +716,6 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -953,7 +916,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1092,10 +1055,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0822456753887466"/>
-          <c:y val="0.161916771752837"/>
-          <c:w val="0.884281521263973"/>
-          <c:h val="0.635561160151324"/>
+          <c:x val="0.0822508118910817"/>
+          <c:y val="0.161937192584185"/>
+          <c:w val="0.884211841119161"/>
+          <c:h val="0.635515197376718"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1209,11 +1172,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48555775"/>
-        <c:axId val="1703753"/>
+        <c:axId val="10932534"/>
+        <c:axId val="37970813"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48555775"/>
+        <c:axId val="10932534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1280,12 +1243,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1703753"/>
+        <c:crossAx val="37970813"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1703753"/>
+        <c:axId val="37970813"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1360,7 +1323,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48555775"/>
+        <c:crossAx val="10932534"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1520,11 +1483,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="63238531"/>
-        <c:axId val="40640062"/>
+        <c:axId val="48593653"/>
+        <c:axId val="42763885"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63238531"/>
+        <c:axId val="48593653"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,7 +1552,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40640062"/>
+        <c:crossAx val="42763885"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1597,7 +1560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40640062"/>
+        <c:axId val="42763885"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,7 +1634,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63238531"/>
+        <c:crossAx val="48593653"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1831,11 +1794,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="26322078"/>
-        <c:axId val="94155694"/>
+        <c:axId val="7560459"/>
+        <c:axId val="76352887"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26322078"/>
+        <c:axId val="7560459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1900,7 +1863,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94155694"/>
+        <c:crossAx val="76352887"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1908,7 +1871,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94155694"/>
+        <c:axId val="76352887"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1982,7 +1945,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26322078"/>
+        <c:crossAx val="7560459"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2142,11 +2105,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="86803505"/>
-        <c:axId val="88705633"/>
+        <c:axId val="26270183"/>
+        <c:axId val="50004781"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86803505"/>
+        <c:axId val="26270183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2211,7 +2174,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88705633"/>
+        <c:crossAx val="50004781"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2219,7 +2182,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88705633"/>
+        <c:axId val="50004781"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2293,7 +2256,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86803505"/>
+        <c:crossAx val="26270183"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2453,11 +2416,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="99220998"/>
-        <c:axId val="57530776"/>
+        <c:axId val="46726566"/>
+        <c:axId val="40393999"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99220998"/>
+        <c:axId val="46726566"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2522,7 +2485,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57530776"/>
+        <c:crossAx val="40393999"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2530,7 +2493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57530776"/>
+        <c:axId val="40393999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2604,7 +2567,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99220998"/>
+        <c:crossAx val="46726566"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2764,11 +2727,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="4707337"/>
-        <c:axId val="97809155"/>
+        <c:axId val="76500548"/>
+        <c:axId val="23135252"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4707337"/>
+        <c:axId val="76500548"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2833,7 +2796,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97809155"/>
+        <c:crossAx val="23135252"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2841,7 +2804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97809155"/>
+        <c:axId val="23135252"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2915,7 +2878,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4707337"/>
+        <c:crossAx val="76500548"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3075,11 +3038,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="16302730"/>
-        <c:axId val="42934370"/>
+        <c:axId val="32762454"/>
+        <c:axId val="60040270"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="16302730"/>
+        <c:axId val="32762454"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3144,7 +3107,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42934370"/>
+        <c:crossAx val="60040270"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3152,7 +3115,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42934370"/>
+        <c:axId val="60040270"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3226,7 +3189,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16302730"/>
+        <c:crossAx val="32762454"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3264,9 +3227,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3201480</xdr:colOff>
+      <xdr:colOff>3201120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
+      <xdr:rowOff>119520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3274,8 +3237,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9115920" y="265680"/>
-        <a:ext cx="5764320" cy="2854440"/>
+        <a:off x="9115560" y="265680"/>
+        <a:ext cx="5763960" cy="2854080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3299,9 +3262,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3309,8 +3272,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="443880"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="443880"/>
+        <a:ext cx="3747240" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3334,9 +3297,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3344,8 +3307,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="443880"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="443880"/>
+        <a:ext cx="3747240" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3369,9 +3332,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3379,8 +3342,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="443880"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="443880"/>
+        <a:ext cx="3747240" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3404,9 +3367,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3414,8 +3377,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="443880"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="443880"/>
+        <a:ext cx="3747240" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3439,9 +3402,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3449,8 +3412,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="443880"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="443880"/>
+        <a:ext cx="3747240" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3474,9 +3437,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3484,8 +3447,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="443880"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="443880"/>
+        <a:ext cx="3747240" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3517,7 +3480,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.57"/>
@@ -5449,11 +5412,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6437,7 +6400,7 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7396,7 +7359,7 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8355,7 +8318,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9313,7 +9276,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -10272,7 +10235,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>

</xml_diff>